<commit_message>
Add test cases for save methods.
</commit_message>
<xml_diff>
--- a/src/test/resources/Test.xlsx
+++ b/src/test/resources/Test.xlsx
@@ -86,10 +86,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,8 +414,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>